<commit_message>
ConfMatrix and pre Nat
</commit_message>
<xml_diff>
--- a/Plots/PBMC_CM.xlsx
+++ b/Plots/PBMC_CM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
   <si>
     <t>B.cell</t>
   </si>
@@ -157,7 +157,7 @@
         <v>0.9982935153583617</v>
       </c>
       <c r="C2" t="n">
-        <v>9.161704076958314E-4</v>
+        <v>4.580852038479157E-4</v>
       </c>
       <c r="D2" t="n">
         <v>0.0028142589118198874</v>
@@ -169,7 +169,7 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.003676470588235294</v>
+        <v>0.003216911764705882</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -189,10 +189,10 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9628950984883188</v>
+        <v>0.9656436097114063</v>
       </c>
       <c r="D3" t="n">
-        <v>0.025328330206378986</v>
+        <v>0.028142589118198873</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -221,10 +221,10 @@
         <v>0.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03618873110398534</v>
+        <v>0.03344021988089785</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9718574108818011</v>
+        <v>0.9690431519699813</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -233,13 +233,13 @@
         <v>0.0</v>
       </c>
       <c r="G4" t="n">
-        <v>4.5955882352941176E-4</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.020689655172413793</v>
+        <v>0.006896551724137931</v>
       </c>
       <c r="J4" t="n">
         <v>0.0</v>
@@ -294,7 +294,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6491228070175439</v>
+        <v>0.7017543859649122</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -317,7 +317,7 @@
         <v>0.0017064846416382253</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>4.580852038479157E-4</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
@@ -326,13 +326,13 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3508771929824561</v>
+        <v>0.2982456140350877</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9866727941176471</v>
+        <v>0.9871323529411765</v>
       </c>
       <c r="H7" t="n">
-        <v>0.09014084507042254</v>
+        <v>0.08169014084507042</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
@@ -361,10 +361,10 @@
         <v>0.0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.006433823529411764</v>
+        <v>0.006893382352941176</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9098591549295775</v>
+        <v>0.9183098591549296</v>
       </c>
       <c r="I8" t="n">
         <v>0.0</v>
@@ -399,7 +399,7 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9793103448275862</v>
+        <v>0.993103448275862</v>
       </c>
       <c r="J9" t="n">
         <v>0.0</v>
@@ -485,7 +485,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9726962457337884</v>
+        <v>0.9675767918088737</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -520,10 +520,10 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9413650939074668</v>
+        <v>0.945487860742098</v>
       </c>
       <c r="D3" t="n">
-        <v>0.019699812382739212</v>
+        <v>0.021575984990619138</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -532,7 +532,7 @@
         <v>0.0</v>
       </c>
       <c r="G3" t="n">
-        <v>9.191176470588235E-4</v>
+        <v>4.5955882352941176E-4</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -552,10 +552,10 @@
         <v>0.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.024278515803939534</v>
+        <v>0.02244617498854787</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9699812382739212</v>
+        <v>0.9652908067542214</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -570,7 +570,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.006896551724137931</v>
+        <v>0.0</v>
       </c>
       <c r="J4" t="n">
         <v>0.0</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
         <v>0.0</v>
@@ -590,10 +590,10 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F5" t="n">
-        <v>0.631578947368421</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8.532423208191126E-4</v>
+        <v>0.0</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -625,13 +625,13 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.22807017543859648</v>
+        <v>0.6491228070175439</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9728860294117647</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.04507042253521127</v>
+        <v>0.0</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
@@ -642,10 +642,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0</v>
+        <v>8.532423208191126E-4</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -657,13 +657,13 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0</v>
+        <v>0.22807017543859648</v>
       </c>
       <c r="G7" t="n">
-        <v>9.191176470588235E-4</v>
+        <v>0.9659926470588235</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8112676056338028</v>
+        <v>0.036619718309859155</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>0.0</v>
@@ -692,13 +692,13 @@
         <v>0.0</v>
       </c>
       <c r="G8" t="n">
-        <v>4.5955882352941176E-4</v>
+        <v>9.191176470588235E-4</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0</v>
+        <v>0.856338028169014</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9413793103448276</v>
+        <v>0.0</v>
       </c>
       <c r="J8" t="n">
         <v>0.0</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
         <v>0.0</v>
@@ -724,47 +724,79 @@
         <v>0.0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>4.5955882352941176E-4</v>
       </c>
       <c r="H9" t="n">
         <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0</v>
+        <v>0.9655172413793104</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9444444444444444</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.026450511945392493</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.03435639028859368</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.009380863039399626</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.14035087719298245</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.024816176470588234</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.14366197183098592</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.05172413793103448</v>
-      </c>
-      <c r="J10" t="n">
+      <c r="B11" t="n">
+        <v>0.031569965870307165</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0320659642693541</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.012195121951219513</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.12280701754385964</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.03216911764705882</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.10704225352112676</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.034482758620689655</v>
+      </c>
+      <c r="J11" t="n">
         <v>0.05555555555555555</v>
       </c>
     </row>

</xml_diff>